<commit_message>
pengambilan nilai blade system
</commit_message>
<xml_diff>
--- a/XIIRPL1(✿◡‿◡)(✿◡‿◡)(✿◡‿◡)/DATA PRAKTIK XII RPl 1.xlsx
+++ b/XIIRPL1(✿◡‿◡)(✿◡‿◡)(✿◡‿◡)/DATA PRAKTIK XII RPl 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdeSetiyawan)(✿◡‿◡)(✿◡‿◡)\XIIRPL1(✿◡‿◡)(✿◡‿◡)(✿◡‿◡)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C7033F-560D-443B-A528-E5D32A77F4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CD42B38-52EC-4F58-B5B8-49985740DB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$G$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -72,9 +73,6 @@
     <t xml:space="preserve">Halaman </t>
   </si>
   <si>
-    <t>LINK</t>
-  </si>
-  <si>
     <t>@yield('sidebar')</t>
   </si>
   <si>
@@ -208,6 +206,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Wafiq </t>
+  </si>
+  <si>
+    <t>LINK (blade)</t>
   </si>
 </sst>
 </file>
@@ -909,10 +910,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8966E4-2275-4E9F-82CA-974F40DBA593}">
   <dimension ref="D1:O1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="29" t="s">
         <v>2</v>
@@ -948,7 +949,7 @@
       </c>
       <c r="I1" s="27"/>
       <c r="J1" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" s="20"/>
       <c r="L1" s="20"/>
@@ -965,7 +966,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>4</v>
@@ -991,10 +992,10 @@
       <c r="E3" s="12"/>
       <c r="F3" s="24"/>
       <c r="G3" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="14"/>
@@ -1009,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="8">
@@ -1031,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="8">
@@ -1053,7 +1054,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="8">
@@ -1075,7 +1076,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="8">
@@ -1097,7 +1098,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="8">
@@ -1119,7 +1120,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="3">
@@ -1141,7 +1142,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="8">
@@ -1163,7 +1164,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="8">
@@ -1185,7 +1186,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="8">
@@ -1207,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="8">
@@ -1229,7 +1230,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="8">
@@ -1251,7 +1252,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="8">
@@ -1273,7 +1274,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="8">
@@ -1295,7 +1296,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="8">
@@ -1317,7 +1318,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="8">
@@ -1339,7 +1340,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="8">
@@ -1361,7 +1362,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="3">
@@ -1383,7 +1384,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="8">
@@ -1405,7 +1406,7 @@
         <v>19</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="8">
@@ -1427,7 +1428,7 @@
         <v>20</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="3">
@@ -1449,7 +1450,7 @@
         <v>21</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="8">
@@ -1471,7 +1472,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="8">
@@ -1493,7 +1494,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="8">
@@ -1515,7 +1516,7 @@
         <v>24</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="8">
@@ -1537,7 +1538,7 @@
         <v>25</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="8">
@@ -1559,7 +1560,7 @@
         <v>26</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="3">
@@ -1581,7 +1582,7 @@
         <v>27</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="8">
@@ -1603,7 +1604,7 @@
         <v>28</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="8">
@@ -1625,7 +1626,7 @@
         <v>29</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="8">
@@ -1647,7 +1648,7 @@
         <v>30</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="8">
@@ -1669,7 +1670,7 @@
         <v>31</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="8">
@@ -1691,7 +1692,7 @@
         <v>32</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="8">
@@ -1713,7 +1714,7 @@
         <v>33</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="8">
@@ -1735,7 +1736,7 @@
         <v>34</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="8">
@@ -1757,7 +1758,7 @@
         <v>35</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="8">
@@ -1779,7 +1780,7 @@
         <v>36</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="8">
@@ -1879,7 +1880,7 @@
     </row>
     <row r="3" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F3" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
@@ -1951,7 +1952,7 @@
     </row>
     <row r="8" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F8" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="32"/>
@@ -1981,12 +1982,12 @@
     </row>
     <row r="10" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F10" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
       <c r="I10" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
@@ -2251,7 +2252,7 @@
     </row>
     <row r="29" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F29" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>

</xml_diff>

<commit_message>
nilai Link di kelas XII RPL 3
</commit_message>
<xml_diff>
--- a/XIIRPL1(✿◡‿◡)(✿◡‿◡)(✿◡‿◡)/DATA PRAKTIK XII RPl 1.xlsx
+++ b/XIIRPL1(✿◡‿◡)(✿◡‿◡)(✿◡‿◡)/DATA PRAKTIK XII RPl 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdeSetiyawan)(✿◡‿◡)(✿◡‿◡)\XIIRPL1(✿◡‿◡)(✿◡‿◡)(✿◡‿◡)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50B41BD-F9EF-465A-8855-D6A1BB6B23B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302C133D-EED6-44BE-890F-8BE22910177F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
   </bookViews>
@@ -25,17 +25,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -262,6 +251,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0&quot;%&quot;"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -319,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -625,11 +617,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -665,72 +708,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,25 +723,109 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1081,10 +1142,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8966E4-2275-4E9F-82CA-974F40DBA593}">
   <dimension ref="B1:R1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,104 +1168,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="26" t="s">
+      <c r="D1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="15" t="s">
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="29" t="s">
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="R1" s="27" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="C2" s="21"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="21"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="J2" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="M2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="37" t="s">
+      <c r="O2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="P2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="32"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="28"/>
     </row>
     <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="21"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="12"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="28"/>
+      <c r="F3" s="39"/>
       <c r="G3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="14"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="32"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="28"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="13">
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1255,7 +1316,7 @@
       <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="14">
         <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1306,7 +1367,7 @@
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="14">
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1357,7 +1418,7 @@
       <c r="C7" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="14">
         <v>4</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1408,7 +1469,7 @@
       <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="14">
         <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1459,7 +1520,7 @@
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="14">
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -1510,7 +1571,7 @@
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="14">
         <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1561,7 +1622,7 @@
       <c r="C11" s="3">
         <v>2</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="14">
         <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -1612,7 +1673,7 @@
       <c r="C12" s="3">
         <v>1</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="14">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1663,7 +1724,7 @@
       <c r="C13" s="3">
         <v>2</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="14">
         <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1714,7 +1775,7 @@
       <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="14">
         <v>11</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1765,7 +1826,7 @@
       <c r="C15" s="3">
         <v>2</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="14">
         <v>12</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1819,7 +1880,7 @@
       <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="14">
         <v>13</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -1835,10 +1896,10 @@
       <c r="H16" s="11">
         <v>1</v>
       </c>
-      <c r="I16" s="42">
-        <v>0</v>
-      </c>
-      <c r="J16" s="42">
+      <c r="I16" s="18">
+        <v>0</v>
+      </c>
+      <c r="J16" s="18">
         <v>0</v>
       </c>
       <c r="K16" s="11">
@@ -1870,7 +1931,7 @@
       <c r="C17" s="3">
         <v>2</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="14">
         <v>14</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -1921,7 +1982,7 @@
       <c r="C18" s="3">
         <v>1</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="14">
         <v>15</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -1972,7 +2033,7 @@
       <c r="C19" s="3">
         <v>2</v>
       </c>
-      <c r="D19" s="36">
+      <c r="D19" s="14">
         <v>16</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -2023,7 +2084,7 @@
       <c r="C20" s="3">
         <v>1</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="14">
         <v>17</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -2074,7 +2135,7 @@
       <c r="C21" s="3">
         <v>2</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="14">
         <v>18</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -2128,7 +2189,7 @@
       <c r="C22" s="3">
         <v>1</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="14">
         <v>19</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -2144,10 +2205,10 @@
       <c r="H22" s="11">
         <v>1</v>
       </c>
-      <c r="I22" s="42">
-        <v>0</v>
-      </c>
-      <c r="J22" s="42">
+      <c r="I22" s="18">
+        <v>0</v>
+      </c>
+      <c r="J22" s="18">
         <v>0</v>
       </c>
       <c r="K22" s="11">
@@ -2179,7 +2240,7 @@
       <c r="C23" s="3">
         <v>2</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="14">
         <v>20</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -2230,7 +2291,7 @@
       <c r="C24" s="3">
         <v>1</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="14">
         <v>21</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -2281,7 +2342,7 @@
       <c r="C25" s="3">
         <v>2</v>
       </c>
-      <c r="D25" s="36">
+      <c r="D25" s="14">
         <v>22</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -2332,7 +2393,7 @@
       <c r="C26" s="3">
         <v>1</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="14">
         <v>23</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -2383,7 +2444,7 @@
       <c r="C27" s="3">
         <v>2</v>
       </c>
-      <c r="D27" s="36">
+      <c r="D27" s="14">
         <v>24</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -2434,7 +2495,7 @@
       <c r="C28" s="3">
         <v>1</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D28" s="14">
         <v>25</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -2485,7 +2546,7 @@
       <c r="C29" s="3">
         <v>2</v>
       </c>
-      <c r="D29" s="36">
+      <c r="D29" s="14">
         <v>26</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -2536,7 +2597,7 @@
       <c r="C30" s="3">
         <v>1</v>
       </c>
-      <c r="D30" s="36">
+      <c r="D30" s="14">
         <v>27</v>
       </c>
       <c r="E30" s="4" t="s">
@@ -2587,7 +2648,7 @@
       <c r="C31" s="3">
         <v>2</v>
       </c>
-      <c r="D31" s="36">
+      <c r="D31" s="14">
         <v>28</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -2638,7 +2699,7 @@
       <c r="C32" s="3">
         <v>1</v>
       </c>
-      <c r="D32" s="36">
+      <c r="D32" s="14">
         <v>29</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -2689,7 +2750,7 @@
       <c r="C33" s="3">
         <v>2</v>
       </c>
-      <c r="D33" s="36">
+      <c r="D33" s="14">
         <v>30</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -2740,7 +2801,7 @@
       <c r="C34" s="3">
         <v>1</v>
       </c>
-      <c r="D34" s="36">
+      <c r="D34" s="14">
         <v>31</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -2791,7 +2852,7 @@
       <c r="C35" s="3">
         <v>2</v>
       </c>
-      <c r="D35" s="36">
+      <c r="D35" s="14">
         <v>32</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -2842,7 +2903,7 @@
       <c r="C36" s="3">
         <v>1</v>
       </c>
-      <c r="D36" s="36">
+      <c r="D36" s="14">
         <v>33</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -2893,7 +2954,7 @@
       <c r="C37" s="3">
         <v>2</v>
       </c>
-      <c r="D37" s="36">
+      <c r="D37" s="14">
         <v>34</v>
       </c>
       <c r="E37" s="4" t="s">
@@ -2944,7 +3005,7 @@
       <c r="C38" s="3">
         <v>1</v>
       </c>
-      <c r="D38" s="36">
+      <c r="D38" s="14">
         <v>35</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -2995,7 +3056,7 @@
       <c r="C39" s="3">
         <v>2</v>
       </c>
-      <c r="D39" s="36">
+      <c r="D39" s="14">
         <v>36</v>
       </c>
       <c r="E39" s="4" t="s">
@@ -3042,11 +3103,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="G40" s="51">
+        <f>(AVERAGE(G4:G39)*100)</f>
+        <v>100</v>
+      </c>
+      <c r="H40" s="52">
+        <f t="shared" ref="H40:J40" si="1">(AVERAGE(H4:H39)*100)</f>
+        <v>100</v>
+      </c>
+      <c r="I40" s="52">
+        <f t="shared" si="1"/>
+        <v>79.861111111111114</v>
+      </c>
+      <c r="J40" s="53">
+        <f t="shared" si="1"/>
+        <v>80.555555555555557</v>
+      </c>
+      <c r="K40" s="50"/>
+      <c r="L40" s="50"/>
+      <c r="M40" s="50"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="50"/>
+      <c r="P40" s="50"/>
+      <c r="Q40" s="50"/>
+      <c r="R40" s="50"/>
+    </row>
+    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="G41" s="54">
+        <f>AVERAGE(G40:J40)</f>
+        <v>90.104166666666657</v>
+      </c>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="56"/>
+    </row>
     <row r="1048576" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G1048576" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="G41:J41"/>
     <mergeCell ref="Q1:Q3"/>
     <mergeCell ref="R1:R3"/>
     <mergeCell ref="C1:C3"/>
@@ -3115,51 +3212,51 @@
   <sheetData>
     <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="44"/>
-      <c r="D3" s="45" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="45" t="s">
+      <c r="E3" s="21"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="46"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="20" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="48"/>
-      <c r="D5" s="45" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="49"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="45" t="s">
+      <c r="E5" s="24"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="49"/>
+      <c r="I5" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3180,31 +3277,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="S1" s="25" t="s">
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="S1" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
     </row>
     <row r="2" spans="6:30" x14ac:dyDescent="0.25">
       <c r="F2" s="2"/>
@@ -3221,767 +3318,767 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="S3" s="40" t="s">
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="S3" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
-      <c r="X3" s="41"/>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="41"/>
-      <c r="AA3" s="41"/>
-      <c r="AB3" s="41"/>
-      <c r="AC3" s="41"/>
-      <c r="AD3" s="41"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="47"/>
+      <c r="AD3" s="47"/>
     </row>
     <row r="4" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="41"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="41"/>
-      <c r="AA4" s="41"/>
-      <c r="AB4" s="41"/>
-      <c r="AC4" s="41"/>
-      <c r="AD4" s="41"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="47"/>
+      <c r="AD4" s="47"/>
     </row>
     <row r="5" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="41"/>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="41"/>
-      <c r="AA5" s="41"/>
-      <c r="AB5" s="41"/>
-      <c r="AC5" s="41"/>
-      <c r="AD5" s="41"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="47"/>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
     </row>
     <row r="6" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="41"/>
-      <c r="AC6" s="41"/>
-      <c r="AD6" s="41"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="47"/>
+      <c r="W6" s="47"/>
+      <c r="X6" s="47"/>
+      <c r="Y6" s="47"/>
+      <c r="Z6" s="47"/>
+      <c r="AA6" s="47"/>
+      <c r="AB6" s="47"/>
+      <c r="AC6" s="47"/>
+      <c r="AD6" s="47"/>
     </row>
     <row r="7" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="41"/>
-      <c r="V7" s="41"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="41"/>
-      <c r="AC7" s="41"/>
-      <c r="AD7" s="41"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="47"/>
+      <c r="W7" s="47"/>
+      <c r="X7" s="47"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="47"/>
+      <c r="AA7" s="47"/>
+      <c r="AB7" s="47"/>
+      <c r="AC7" s="47"/>
+      <c r="AD7" s="47"/>
     </row>
     <row r="8" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="S8" s="40" t="s">
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="S8" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="T8" s="41"/>
-      <c r="U8" s="41"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="41"/>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
-      <c r="AB8" s="41"/>
-      <c r="AC8" s="41"/>
-      <c r="AD8" s="41"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="47"/>
+      <c r="X8" s="47"/>
+      <c r="Y8" s="47"/>
+      <c r="Z8" s="47"/>
+      <c r="AA8" s="47"/>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="47"/>
+      <c r="AD8" s="47"/>
     </row>
     <row r="9" spans="6:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="41"/>
-      <c r="U9" s="41"/>
-      <c r="V9" s="41"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="41"/>
-      <c r="AA9" s="41"/>
-      <c r="AB9" s="41"/>
-      <c r="AC9" s="41"/>
-      <c r="AD9" s="41"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
+      <c r="V9" s="47"/>
+      <c r="W9" s="47"/>
+      <c r="X9" s="47"/>
+      <c r="Y9" s="47"/>
+      <c r="Z9" s="47"/>
+      <c r="AA9" s="47"/>
+      <c r="AB9" s="47"/>
+      <c r="AC9" s="47"/>
+      <c r="AD9" s="47"/>
     </row>
     <row r="10" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="22" t="s">
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="S10" s="40" t="s">
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="S10" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="T10" s="41"/>
-      <c r="U10" s="41"/>
-      <c r="V10" s="40" t="s">
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="41"/>
-      <c r="AB10" s="41"/>
-      <c r="AC10" s="41"/>
-      <c r="AD10" s="41"/>
+      <c r="W10" s="47"/>
+      <c r="X10" s="47"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="47"/>
+      <c r="AA10" s="47"/>
+      <c r="AB10" s="47"/>
+      <c r="AC10" s="47"/>
+      <c r="AD10" s="47"/>
     </row>
     <row r="11" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="41"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="41"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="41"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="41"/>
-      <c r="AB11" s="41"/>
-      <c r="AC11" s="41"/>
-      <c r="AD11" s="41"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="47"/>
+      <c r="W11" s="47"/>
+      <c r="X11" s="47"/>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="47"/>
+      <c r="AA11" s="47"/>
+      <c r="AB11" s="47"/>
+      <c r="AC11" s="47"/>
+      <c r="AD11" s="47"/>
     </row>
     <row r="12" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="41"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="41"/>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="41"/>
-      <c r="AC12" s="41"/>
-      <c r="AD12" s="41"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="47"/>
+      <c r="W12" s="47"/>
+      <c r="X12" s="47"/>
+      <c r="Y12" s="47"/>
+      <c r="Z12" s="47"/>
+      <c r="AA12" s="47"/>
+      <c r="AB12" s="47"/>
+      <c r="AC12" s="47"/>
+      <c r="AD12" s="47"/>
     </row>
     <row r="13" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="41"/>
-      <c r="AC13" s="41"/>
-      <c r="AD13" s="41"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="47"/>
+      <c r="W13" s="47"/>
+      <c r="X13" s="47"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="47"/>
+      <c r="AB13" s="47"/>
+      <c r="AC13" s="47"/>
+      <c r="AD13" s="47"/>
     </row>
     <row r="14" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="41"/>
-      <c r="Y14" s="41"/>
-      <c r="Z14" s="41"/>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="41"/>
-      <c r="AC14" s="41"/>
-      <c r="AD14" s="41"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="S14" s="47"/>
+      <c r="T14" s="47"/>
+      <c r="U14" s="47"/>
+      <c r="V14" s="47"/>
+      <c r="W14" s="47"/>
+      <c r="X14" s="47"/>
+      <c r="Y14" s="47"/>
+      <c r="Z14" s="47"/>
+      <c r="AA14" s="47"/>
+      <c r="AB14" s="47"/>
+      <c r="AC14" s="47"/>
+      <c r="AD14" s="47"/>
     </row>
     <row r="15" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="S15" s="41"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="41"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="41"/>
-      <c r="AC15" s="41"/>
-      <c r="AD15" s="41"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="47"/>
+      <c r="V15" s="47"/>
+      <c r="W15" s="47"/>
+      <c r="X15" s="47"/>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="47"/>
+      <c r="AA15" s="47"/>
+      <c r="AB15" s="47"/>
+      <c r="AC15" s="47"/>
+      <c r="AD15" s="47"/>
     </row>
     <row r="16" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="S16" s="41"/>
-      <c r="T16" s="41"/>
-      <c r="U16" s="41"/>
-      <c r="V16" s="41"/>
-      <c r="W16" s="41"/>
-      <c r="X16" s="41"/>
-      <c r="Y16" s="41"/>
-      <c r="Z16" s="41"/>
-      <c r="AA16" s="41"/>
-      <c r="AB16" s="41"/>
-      <c r="AC16" s="41"/>
-      <c r="AD16" s="41"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="47"/>
+      <c r="V16" s="47"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="47"/>
+      <c r="Y16" s="47"/>
+      <c r="Z16" s="47"/>
+      <c r="AA16" s="47"/>
+      <c r="AB16" s="47"/>
+      <c r="AC16" s="47"/>
+      <c r="AD16" s="47"/>
     </row>
     <row r="17" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="S17" s="41"/>
-      <c r="T17" s="41"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="41"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="41"/>
-      <c r="Y17" s="41"/>
-      <c r="Z17" s="41"/>
-      <c r="AA17" s="41"/>
-      <c r="AB17" s="41"/>
-      <c r="AC17" s="41"/>
-      <c r="AD17" s="41"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="47"/>
+      <c r="AA17" s="47"/>
+      <c r="AB17" s="47"/>
+      <c r="AC17" s="47"/>
+      <c r="AD17" s="47"/>
     </row>
     <row r="18" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="41"/>
-      <c r="U18" s="41"/>
-      <c r="V18" s="41"/>
-      <c r="W18" s="41"/>
-      <c r="X18" s="41"/>
-      <c r="Y18" s="41"/>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="41"/>
-      <c r="AB18" s="41"/>
-      <c r="AC18" s="41"/>
-      <c r="AD18" s="41"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="S18" s="47"/>
+      <c r="T18" s="47"/>
+      <c r="U18" s="47"/>
+      <c r="V18" s="47"/>
+      <c r="W18" s="47"/>
+      <c r="X18" s="47"/>
+      <c r="Y18" s="47"/>
+      <c r="Z18" s="47"/>
+      <c r="AA18" s="47"/>
+      <c r="AB18" s="47"/>
+      <c r="AC18" s="47"/>
+      <c r="AD18" s="47"/>
     </row>
     <row r="19" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="41"/>
-      <c r="U19" s="41"/>
-      <c r="V19" s="41"/>
-      <c r="W19" s="41"/>
-      <c r="X19" s="41"/>
-      <c r="Y19" s="41"/>
-      <c r="Z19" s="41"/>
-      <c r="AA19" s="41"/>
-      <c r="AB19" s="41"/>
-      <c r="AC19" s="41"/>
-      <c r="AD19" s="41"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="49"/>
+      <c r="S19" s="47"/>
+      <c r="T19" s="47"/>
+      <c r="U19" s="47"/>
+      <c r="V19" s="47"/>
+      <c r="W19" s="47"/>
+      <c r="X19" s="47"/>
+      <c r="Y19" s="47"/>
+      <c r="Z19" s="47"/>
+      <c r="AA19" s="47"/>
+      <c r="AB19" s="47"/>
+      <c r="AC19" s="47"/>
+      <c r="AD19" s="47"/>
     </row>
     <row r="20" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="41"/>
-      <c r="U20" s="41"/>
-      <c r="V20" s="41"/>
-      <c r="W20" s="41"/>
-      <c r="X20" s="41"/>
-      <c r="Y20" s="41"/>
-      <c r="Z20" s="41"/>
-      <c r="AA20" s="41"/>
-      <c r="AB20" s="41"/>
-      <c r="AC20" s="41"/>
-      <c r="AD20" s="41"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="49"/>
+      <c r="S20" s="47"/>
+      <c r="T20" s="47"/>
+      <c r="U20" s="47"/>
+      <c r="V20" s="47"/>
+      <c r="W20" s="47"/>
+      <c r="X20" s="47"/>
+      <c r="Y20" s="47"/>
+      <c r="Z20" s="47"/>
+      <c r="AA20" s="47"/>
+      <c r="AB20" s="47"/>
+      <c r="AC20" s="47"/>
+      <c r="AD20" s="47"/>
     </row>
     <row r="21" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="S21" s="41"/>
-      <c r="T21" s="41"/>
-      <c r="U21" s="41"/>
-      <c r="V21" s="41"/>
-      <c r="W21" s="41"/>
-      <c r="X21" s="41"/>
-      <c r="Y21" s="41"/>
-      <c r="Z21" s="41"/>
-      <c r="AA21" s="41"/>
-      <c r="AB21" s="41"/>
-      <c r="AC21" s="41"/>
-      <c r="AD21" s="41"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="49"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="47"/>
+      <c r="V21" s="47"/>
+      <c r="W21" s="47"/>
+      <c r="X21" s="47"/>
+      <c r="Y21" s="47"/>
+      <c r="Z21" s="47"/>
+      <c r="AA21" s="47"/>
+      <c r="AB21" s="47"/>
+      <c r="AC21" s="47"/>
+      <c r="AD21" s="47"/>
     </row>
     <row r="22" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="S22" s="41"/>
-      <c r="T22" s="41"/>
-      <c r="U22" s="41"/>
-      <c r="V22" s="41"/>
-      <c r="W22" s="41"/>
-      <c r="X22" s="41"/>
-      <c r="Y22" s="41"/>
-      <c r="Z22" s="41"/>
-      <c r="AA22" s="41"/>
-      <c r="AB22" s="41"/>
-      <c r="AC22" s="41"/>
-      <c r="AD22" s="41"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="49"/>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="49"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
+      <c r="U22" s="47"/>
+      <c r="V22" s="47"/>
+      <c r="W22" s="47"/>
+      <c r="X22" s="47"/>
+      <c r="Y22" s="47"/>
+      <c r="Z22" s="47"/>
+      <c r="AA22" s="47"/>
+      <c r="AB22" s="47"/>
+      <c r="AC22" s="47"/>
+      <c r="AD22" s="47"/>
     </row>
     <row r="23" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="S23" s="41"/>
-      <c r="T23" s="41"/>
-      <c r="U23" s="41"/>
-      <c r="V23" s="41"/>
-      <c r="W23" s="41"/>
-      <c r="X23" s="41"/>
-      <c r="Y23" s="41"/>
-      <c r="Z23" s="41"/>
-      <c r="AA23" s="41"/>
-      <c r="AB23" s="41"/>
-      <c r="AC23" s="41"/>
-      <c r="AD23" s="41"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="S23" s="47"/>
+      <c r="T23" s="47"/>
+      <c r="U23" s="47"/>
+      <c r="V23" s="47"/>
+      <c r="W23" s="47"/>
+      <c r="X23" s="47"/>
+      <c r="Y23" s="47"/>
+      <c r="Z23" s="47"/>
+      <c r="AA23" s="47"/>
+      <c r="AB23" s="47"/>
+      <c r="AC23" s="47"/>
+      <c r="AD23" s="47"/>
     </row>
     <row r="24" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="S24" s="41"/>
-      <c r="T24" s="41"/>
-      <c r="U24" s="41"/>
-      <c r="V24" s="41"/>
-      <c r="W24" s="41"/>
-      <c r="X24" s="41"/>
-      <c r="Y24" s="41"/>
-      <c r="Z24" s="41"/>
-      <c r="AA24" s="41"/>
-      <c r="AB24" s="41"/>
-      <c r="AC24" s="41"/>
-      <c r="AD24" s="41"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
+      <c r="S24" s="47"/>
+      <c r="T24" s="47"/>
+      <c r="U24" s="47"/>
+      <c r="V24" s="47"/>
+      <c r="W24" s="47"/>
+      <c r="X24" s="47"/>
+      <c r="Y24" s="47"/>
+      <c r="Z24" s="47"/>
+      <c r="AA24" s="47"/>
+      <c r="AB24" s="47"/>
+      <c r="AC24" s="47"/>
+      <c r="AD24" s="47"/>
     </row>
     <row r="25" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="S25" s="41"/>
-      <c r="T25" s="41"/>
-      <c r="U25" s="41"/>
-      <c r="V25" s="41"/>
-      <c r="W25" s="41"/>
-      <c r="X25" s="41"/>
-      <c r="Y25" s="41"/>
-      <c r="Z25" s="41"/>
-      <c r="AA25" s="41"/>
-      <c r="AB25" s="41"/>
-      <c r="AC25" s="41"/>
-      <c r="AD25" s="41"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="49"/>
+      <c r="S25" s="47"/>
+      <c r="T25" s="47"/>
+      <c r="U25" s="47"/>
+      <c r="V25" s="47"/>
+      <c r="W25" s="47"/>
+      <c r="X25" s="47"/>
+      <c r="Y25" s="47"/>
+      <c r="Z25" s="47"/>
+      <c r="AA25" s="47"/>
+      <c r="AB25" s="47"/>
+      <c r="AC25" s="47"/>
+      <c r="AD25" s="47"/>
     </row>
     <row r="26" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="S26" s="41"/>
-      <c r="T26" s="41"/>
-      <c r="U26" s="41"/>
-      <c r="V26" s="41"/>
-      <c r="W26" s="41"/>
-      <c r="X26" s="41"/>
-      <c r="Y26" s="41"/>
-      <c r="Z26" s="41"/>
-      <c r="AA26" s="41"/>
-      <c r="AB26" s="41"/>
-      <c r="AC26" s="41"/>
-      <c r="AD26" s="41"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="47"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="47"/>
+      <c r="Y26" s="47"/>
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="47"/>
+      <c r="AD26" s="47"/>
     </row>
     <row r="27" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="23"/>
-      <c r="S27" s="41"/>
-      <c r="T27" s="41"/>
-      <c r="U27" s="41"/>
-      <c r="V27" s="41"/>
-      <c r="W27" s="41"/>
-      <c r="X27" s="41"/>
-      <c r="Y27" s="41"/>
-      <c r="Z27" s="41"/>
-      <c r="AA27" s="41"/>
-      <c r="AB27" s="41"/>
-      <c r="AC27" s="41"/>
-      <c r="AD27" s="41"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="49"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="49"/>
+      <c r="S27" s="47"/>
+      <c r="T27" s="47"/>
+      <c r="U27" s="47"/>
+      <c r="V27" s="47"/>
+      <c r="W27" s="47"/>
+      <c r="X27" s="47"/>
+      <c r="Y27" s="47"/>
+      <c r="Z27" s="47"/>
+      <c r="AA27" s="47"/>
+      <c r="AB27" s="47"/>
+      <c r="AC27" s="47"/>
+      <c r="AD27" s="47"/>
     </row>
     <row r="28" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="S28" s="41"/>
-      <c r="T28" s="41"/>
-      <c r="U28" s="41"/>
-      <c r="V28" s="41"/>
-      <c r="W28" s="41"/>
-      <c r="X28" s="41"/>
-      <c r="Y28" s="41"/>
-      <c r="Z28" s="41"/>
-      <c r="AA28" s="41"/>
-      <c r="AB28" s="41"/>
-      <c r="AC28" s="41"/>
-      <c r="AD28" s="41"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="S28" s="47"/>
+      <c r="T28" s="47"/>
+      <c r="U28" s="47"/>
+      <c r="V28" s="47"/>
+      <c r="W28" s="47"/>
+      <c r="X28" s="47"/>
+      <c r="Y28" s="47"/>
+      <c r="Z28" s="47"/>
+      <c r="AA28" s="47"/>
+      <c r="AB28" s="47"/>
+      <c r="AC28" s="47"/>
+      <c r="AD28" s="47"/>
     </row>
     <row r="29" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="S29" s="40" t="s">
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="49"/>
+      <c r="S29" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="T29" s="41"/>
-      <c r="U29" s="41"/>
-      <c r="V29" s="41"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="41"/>
-      <c r="Y29" s="41"/>
-      <c r="Z29" s="41"/>
-      <c r="AA29" s="41"/>
-      <c r="AB29" s="41"/>
-      <c r="AC29" s="41"/>
-      <c r="AD29" s="41"/>
+      <c r="T29" s="47"/>
+      <c r="U29" s="47"/>
+      <c r="V29" s="47"/>
+      <c r="W29" s="47"/>
+      <c r="X29" s="47"/>
+      <c r="Y29" s="47"/>
+      <c r="Z29" s="47"/>
+      <c r="AA29" s="47"/>
+      <c r="AB29" s="47"/>
+      <c r="AC29" s="47"/>
+      <c r="AD29" s="47"/>
     </row>
     <row r="30" spans="6:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="23"/>
-      <c r="S30" s="41"/>
-      <c r="T30" s="41"/>
-      <c r="U30" s="41"/>
-      <c r="V30" s="41"/>
-      <c r="W30" s="41"/>
-      <c r="X30" s="41"/>
-      <c r="Y30" s="41"/>
-      <c r="Z30" s="41"/>
-      <c r="AA30" s="41"/>
-      <c r="AB30" s="41"/>
-      <c r="AC30" s="41"/>
-      <c r="AD30" s="41"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="S30" s="47"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="47"/>
+      <c r="V30" s="47"/>
+      <c r="W30" s="47"/>
+      <c r="X30" s="47"/>
+      <c r="Y30" s="47"/>
+      <c r="Z30" s="47"/>
+      <c r="AA30" s="47"/>
+      <c r="AB30" s="47"/>
+      <c r="AC30" s="47"/>
+      <c r="AD30" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="S29:AD30"/>
+    <mergeCell ref="F3:Q7"/>
+    <mergeCell ref="F8:Q9"/>
+    <mergeCell ref="F10:H28"/>
+    <mergeCell ref="I10:Q28"/>
+    <mergeCell ref="F29:Q30"/>
     <mergeCell ref="H1:P1"/>
     <mergeCell ref="S1:AD1"/>
     <mergeCell ref="S3:AD7"/>
     <mergeCell ref="S8:AD9"/>
     <mergeCell ref="S10:U28"/>
     <mergeCell ref="V10:AD28"/>
-    <mergeCell ref="S29:AD30"/>
-    <mergeCell ref="F3:Q7"/>
-    <mergeCell ref="F8:Q9"/>
-    <mergeCell ref="F10:H28"/>
-    <mergeCell ref="I10:Q28"/>
-    <mergeCell ref="F29:Q30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>